<commit_message>
fix(excel): properly handling ion number format retrieved as Long, BigDecimal or BigIntegers
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/insurance_sample.xlsx
+++ b/src/test/resources/excel/insurance_sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t xml:space="preserve">policyID</t>
   </si>
@@ -79,30 +79,50 @@
     <t xml:space="preserve">date</t>
   </si>
   <si>
+    <t xml:space="preserve">119736</t>
+  </si>
+  <si>
     <t xml:space="preserve">FL</t>
   </si>
   <si>
     <t xml:space="preserve">CLAY COUNTY</t>
   </si>
   <si>
+    <t xml:space="preserve">9223372036854775808</t>
+  </si>
+  <si>
     <t xml:space="preserve">Residential</t>
   </si>
   <si>
     <t xml:space="preserve">Masonry</t>
   </si>
   <si>
+    <t xml:space="preserve">448094</t>
+  </si>
+  <si>
+    <t xml:space="preserve">206893</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">333743</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172534</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="0.00E+00"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -124,6 +144,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2AACB8"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -168,12 +194,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -186,6 +224,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF2AACB8"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -197,17 +295,17 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S3" activeCellId="0" sqref="S3"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.15"/>
@@ -222,8 +320,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.04"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -282,20 +380,20 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>119736</v>
+      <c r="A2" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>498960</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>498960</v>
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>922337203685478</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>498960</v>
@@ -328,27 +426,27 @@
         <v>-81.711777</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="R2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S2" s="1" t="n">
+      <c r="S2" s="4" t="n">
         <v>45083</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>448094</v>
+      <c r="A3" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1322376.3</v>
@@ -387,27 +485,27 @@
         <v>-81.707664</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="R3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="S3" s="1" t="n">
+      <c r="S3" s="4" t="n">
         <v>45119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>206893</v>
+      <c r="A4" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>190724.4</v>
@@ -446,27 +544,27 @@
         <v>-81.700455</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="R4" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S4" s="1" t="n">
+      <c r="S4" s="4" t="n">
         <v>45160</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>333743</v>
+      <c r="A5" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0</v>
@@ -505,27 +603,27 @@
         <v>-81.707703</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="R5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="S5" s="1" t="n">
+      <c r="S5" s="4" t="n">
         <v>45353</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>172534</v>
+      <c r="A6" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>0</v>
@@ -564,15 +662,15 @@
         <v>-81.702675</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="R6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="S6" s="1" t="n">
+      <c r="S6" s="4" t="n">
         <v>45292</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix(excel-ion): handle formulas properly
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/insurance_sample.xlsx
+++ b/src/test/resources/excel/insurance_sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t xml:space="preserve">policyID</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t xml:space="preserve">FL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLAY COUNTY</t>
   </si>
   <si>
     <t xml:space="preserve">9223372036854775808</t>
@@ -150,6 +147,7 @@
       <color rgb="FF2AACB8"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -295,10 +293,10 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.61328125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.79"/>
@@ -386,14 +384,15 @@
       <c r="B2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>21</v>
+      <c r="C2" s="0" t="str">
+        <f aca="false">UPPER("clay county")</f>
+        <v>CLAY COUNTY</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>922337203685478</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>498960</v>
@@ -426,10 +425,10 @@
         <v>-81.711777</v>
       </c>
       <c r="P2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="R2" s="0" t="n">
         <v>1</v>
@@ -440,13 +439,14 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>21</v>
+      <c r="C3" s="0" t="str">
+        <f aca="false">UPPER("clay county")</f>
+        <v>CLAY COUNTY</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1322376.3</v>
@@ -485,10 +485,10 @@
         <v>-81.707664</v>
       </c>
       <c r="P3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>24</v>
       </c>
       <c r="R3" s="0" t="n">
         <v>3</v>
@@ -499,13 +499,14 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>21</v>
+      <c r="C4" s="0" t="str">
+        <f aca="false">UPPER("clay county")</f>
+        <v>CLAY COUNTY</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>190724.4</v>
@@ -544,10 +545,10 @@
         <v>-81.700455</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R4" s="0" t="n">
         <v>1</v>
@@ -558,13 +559,14 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>21</v>
+      <c r="C5" s="0" t="str">
+        <f aca="false">UPPER("clay county")</f>
+        <v>CLAY COUNTY</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0</v>
@@ -603,10 +605,10 @@
         <v>-81.707703</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R5" s="0" t="n">
         <v>3</v>
@@ -617,13 +619,14 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>21</v>
+      <c r="C6" s="0" t="str">
+        <f aca="false">UPPER("clay county")</f>
+        <v>CLAY COUNTY</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>0</v>
@@ -662,10 +665,10 @@
         <v>-81.702675</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="R6" s="0" t="n">
         <v>1</v>

</xml_diff>